<commit_message>
Update test fixture to match new schema.
</commit_message>
<xml_diff>
--- a/tests/fixtures/verbal-conjugation.xlsx
+++ b/tests/fixtures/verbal-conjugation.xlsx
@@ -175,18 +175,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> son regulares de la 1ª conjugación. modelo. Conjug. </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">trobar</t>
+      <t xml:space="preserve"> son regulares de la 1ª conjugación. modelo. Conjug. t</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">robar (hallar)</t>
     </r>
   </si>
 </sst>
@@ -332,7 +332,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,7 +362,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="27.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="40.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>